<commit_message>
SmartClockWeb32: TFT_eSPI -> DISABLE_ALL_LIBRARY_WARNINGS
</commit_message>
<xml_diff>
--- a/arduino/ФСА для ALI магазин.xlsx
+++ b/arduino/ФСА для ALI магазин.xlsx
@@ -1,26 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arduino\arduino\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A94B20-A983-4491-952A-E34641F4B1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="12435" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="магазины" sheetId="1" r:id="rId1"/>
     <sheet name="изделия" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>VLaskin</author>
   </authors>
   <commentList>
-    <comment ref="J16" authorId="0">
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -39,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>GREAT WALL Electronics Co., Ltd.</t>
   </si>
@@ -177,13 +195,28 @@
   </si>
   <si>
     <t>сервопривод (360°)</t>
+  </si>
+  <si>
+    <t>Всего доступно  байт.</t>
+  </si>
+  <si>
+    <t>Глобальные переменные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Скетч использует </t>
+  </si>
+  <si>
+    <t>Памяти устройства</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +268,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -274,7 +323,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -593,6 +642,80 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -600,7 +723,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -677,25 +800,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -740,25 +848,60 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -766,14 +909,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -811,9 +957,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -846,9 +992,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -881,9 +1044,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1056,7 +1236,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1078,21 +1258,21 @@
   <sheetData>
     <row r="1" spans="2:13" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="34"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="54"/>
       <c r="M2" s="27" t="s">
         <v>9</v>
       </c>
@@ -1102,22 +1282,22 @@
       <c r="C3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="28" t="s">
+      <c r="E3" s="57"/>
+      <c r="F3" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="28" t="s">
+      <c r="G3" s="57"/>
+      <c r="H3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="28" t="s">
+      <c r="I3" s="56"/>
+      <c r="J3" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="30"/>
+      <c r="K3" s="57"/>
       <c r="L3" s="26" t="s">
         <v>21</v>
       </c>
@@ -1539,18 +1719,18 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="http://ru.aliexpress.com/store/721071"/>
-    <hyperlink ref="B5" r:id="rId2" tooltip="GREAT WALL Electronics Co., Ltd." display="http://www.aliexpress.com/store/731260"/>
-    <hyperlink ref="B7" r:id="rId3" tooltip="A+A+A+" display="http://www.aliexpress.com/store/110055"/>
-    <hyperlink ref="B8" r:id="rId4" display="http://ru.aliexpress.com/store/535576"/>
-    <hyperlink ref="B9" r:id="rId5" tooltip="Corn Green" display="http://ru.aliexpress.com/store/1905393"/>
-    <hyperlink ref="B10" r:id="rId6" display="http://ru.aliexpress.com/store/1337009"/>
-    <hyperlink ref="B11" r:id="rId7" display="http://ru.aliexpress.com/store/1630603"/>
-    <hyperlink ref="B12" r:id="rId8" display="http://ru.aliexpress.com/store/403088"/>
-    <hyperlink ref="B13" r:id="rId9" display="http://ru.aliexpress.com/store/1757110"/>
-    <hyperlink ref="B14" r:id="rId10" display="http://ru.aliexpress.com/store/1516062"/>
-    <hyperlink ref="B15" r:id="rId11" display="http://ru.aliexpress.com/store/1182157"/>
-    <hyperlink ref="B16" r:id="rId12" display="http://ru.aliexpress.com/store/214486"/>
+    <hyperlink ref="B6" r:id="rId1" display="http://ru.aliexpress.com/store/721071" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B5" r:id="rId2" tooltip="GREAT WALL Electronics Co., Ltd." display="http://www.aliexpress.com/store/731260" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B7" r:id="rId3" tooltip="A+A+A+" display="http://www.aliexpress.com/store/110055" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" display="http://ru.aliexpress.com/store/535576" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" tooltip="Corn Green" display="http://ru.aliexpress.com/store/1905393" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" display="http://ru.aliexpress.com/store/1337009" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" display="http://ru.aliexpress.com/store/1630603" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" display="http://ru.aliexpress.com/store/403088" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" display="http://ru.aliexpress.com/store/1757110" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B14" r:id="rId10" display="http://ru.aliexpress.com/store/1516062" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B15" r:id="rId11" display="http://ru.aliexpress.com/store/1182157" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B16" r:id="rId12" display="http://ru.aliexpress.com/store/214486" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId13"/>
@@ -1559,10 +1739,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="B2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1578,176 +1758,506 @@
   <sheetData>
     <row r="1" spans="2:6" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="34" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="35">
         <v>90</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="40" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="56"/>
-      <c r="C4" s="53" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="42">
         <v>180</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="43" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="36">
         <v>350</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="39" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="41">
+      <c r="D6" s="36">
         <v>550</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="39" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="58"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="44"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="39"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="58"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="44"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="39"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="58"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="44"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="39"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="58"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="44"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="39"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="58"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="44"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="39"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="58"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="44"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="39"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="58"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="44"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="39"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="58"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="44"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="39"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="58"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="44"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="39"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="58"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="44"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="39"/>
     </row>
     <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="59"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="46"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:B4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
-    <hyperlink ref="B3:B4" r:id="rId5" display="сервопривод (180°)"/>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B3:B4" r:id="rId5" display="сервопривод (180°)" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18B4D82-95FA-4E75-A305-7A414E0C2778}">
+  <dimension ref="A1:E39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="67">
+        <v>1310720</v>
+      </c>
+      <c r="D1" s="67">
+        <v>327680</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="64"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="60"/>
+      <c r="B3" s="67">
+        <v>808849</v>
+      </c>
+      <c r="C3" s="65">
+        <f>B3/$B$1</f>
+        <v>0.61710281372070308</v>
+      </c>
+      <c r="D3" s="67">
+        <v>44612</v>
+      </c>
+      <c r="E3" s="65">
+        <f>D3/$D$1</f>
+        <v>0.13614501953124999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="60"/>
+      <c r="B4" s="67">
+        <v>808913</v>
+      </c>
+      <c r="C4" s="65">
+        <f>B4/$B$1</f>
+        <v>0.61715164184570315</v>
+      </c>
+      <c r="D4" s="67">
+        <v>44612</v>
+      </c>
+      <c r="E4" s="65">
+        <f>D4/$D$1</f>
+        <v>0.13614501953124999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="60"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="65"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="60"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="65"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="60"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="65"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="60"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="65"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="60"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="65"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="60"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="65"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="60"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="65"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="60"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="65"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="60"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="65"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="60"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="65"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="60"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="65"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="60"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="65"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="60"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="65"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="60"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="65"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="60"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="65"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="60"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="65"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="60"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="65"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="60"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="65"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="60"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="65"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="60"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="65"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="60"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="65"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="60"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="65"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="60"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="65"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="60"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="65"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="60"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="65"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="60"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="65"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="60"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="65"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="60"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="65"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="60"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="65"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="60"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="65"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="60"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="65"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="60"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="65"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="60"/>
+      <c r="B37" s="67"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="65"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="60"/>
+      <c r="B38" s="67"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="65"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="61"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="66"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="66"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
SmartClockWeb8266: add getBright, GetDatetime, PostDatetime
</commit_message>
<xml_diff>
--- a/arduino/ФСА для ALI магазин.xlsx
+++ b/arduino/ФСА для ALI магазин.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arduino\arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9C44EA-5DB3-4C44-8BA9-C34CBD8A5CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5045009-574D-4810-9D6B-71B9FA4A9A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="магазины" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000%"/>
-    <numFmt numFmtId="170" formatCode="dd/mm/yyyy\ hh:mm"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -784,7 +784,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -940,8 +940,10 @@
     <xf numFmtId="10" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -971,10 +973,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1339,17 +1337,17 @@
         <v>2</v>
       </c>
       <c r="C2" s="29"/>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="64"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="66"/>
       <c r="M2" s="27" t="s">
         <v>9</v>
       </c>
@@ -1359,22 +1357,22 @@
       <c r="C3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="67"/>
-      <c r="F3" s="65" t="s">
+      <c r="E3" s="69"/>
+      <c r="F3" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="67"/>
-      <c r="H3" s="65" t="s">
+      <c r="G3" s="69"/>
+      <c r="H3" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="66"/>
-      <c r="J3" s="65" t="s">
+      <c r="I3" s="68"/>
+      <c r="J3" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="67"/>
+      <c r="K3" s="69"/>
       <c r="L3" s="26" t="s">
         <v>21</v>
       </c>
@@ -1852,7 +1850,7 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="70" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="49" t="s">
@@ -1869,7 +1867,7 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="69"/>
+      <c r="B4" s="71"/>
       <c r="C4" s="48" t="s">
         <v>41</v>
       </c>
@@ -2013,7 +2011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18B4D82-95FA-4E75-A305-7A414E0C2778}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2027,9 +2025,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62">
+      <c r="A1" s="61">
         <f ca="1">NOW()</f>
-        <v>45334.053180439812</v>
+        <v>45335.068531712961</v>
       </c>
       <c r="B1" s="56">
         <v>1310720</v>
@@ -2042,17 +2040,17 @@
       <c r="A2" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70" t="s">
+      <c r="C2" s="72"/>
+      <c r="D2" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="71"/>
+      <c r="E2" s="73"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="75"/>
+      <c r="A3" s="62"/>
       <c r="B3" s="56">
         <v>808849</v>
       </c>
@@ -2069,7 +2067,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="75"/>
+      <c r="A4" s="62"/>
       <c r="B4" s="56">
         <v>808861</v>
       </c>
@@ -2086,7 +2084,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="75">
+      <c r="A5" s="62">
         <v>45331.98609953704</v>
       </c>
       <c r="B5" s="56">
@@ -2105,7 +2103,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="76">
+      <c r="A6" s="63">
         <v>45332.073997569445</v>
       </c>
       <c r="B6" s="56">
@@ -2124,231 +2122,231 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="75"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="56"/>
       <c r="C7" s="54"/>
       <c r="D7" s="56"/>
       <c r="E7" s="54"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="75"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="56"/>
       <c r="C8" s="54"/>
       <c r="D8" s="56"/>
       <c r="E8" s="54"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="75"/>
+      <c r="A9" s="62"/>
       <c r="B9" s="56"/>
       <c r="C9" s="54"/>
       <c r="D9" s="56"/>
       <c r="E9" s="54"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="75"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="56"/>
       <c r="C10" s="54"/>
       <c r="D10" s="56"/>
       <c r="E10" s="54"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="75"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="56"/>
       <c r="C11" s="54"/>
       <c r="D11" s="56"/>
       <c r="E11" s="54"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="75"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="56"/>
       <c r="C12" s="54"/>
       <c r="D12" s="56"/>
       <c r="E12" s="54"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="75"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="56"/>
       <c r="C13" s="54"/>
       <c r="D13" s="56"/>
       <c r="E13" s="54"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="75"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="56"/>
       <c r="C14" s="54"/>
       <c r="D14" s="56"/>
       <c r="E14" s="54"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="75"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="56"/>
       <c r="C15" s="54"/>
       <c r="D15" s="56"/>
       <c r="E15" s="54"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="75"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="56"/>
       <c r="C16" s="54"/>
       <c r="D16" s="56"/>
       <c r="E16" s="54"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="75"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="56"/>
       <c r="C17" s="54"/>
       <c r="D17" s="56"/>
       <c r="E17" s="54"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="75"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="56"/>
       <c r="C18" s="54"/>
       <c r="D18" s="56"/>
       <c r="E18" s="54"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="75"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="56"/>
       <c r="C19" s="54"/>
       <c r="D19" s="56"/>
       <c r="E19" s="54"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="75"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="56"/>
       <c r="C20" s="54"/>
       <c r="D20" s="56"/>
       <c r="E20" s="54"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="75"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="56"/>
       <c r="C21" s="54"/>
       <c r="D21" s="56"/>
       <c r="E21" s="54"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="75"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="56"/>
       <c r="C22" s="54"/>
       <c r="D22" s="56"/>
       <c r="E22" s="54"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="75"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="56"/>
       <c r="C23" s="54"/>
       <c r="D23" s="56"/>
       <c r="E23" s="54"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="75"/>
+      <c r="A24" s="62"/>
       <c r="B24" s="56"/>
       <c r="C24" s="54"/>
       <c r="D24" s="56"/>
       <c r="E24" s="54"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="75"/>
+      <c r="A25" s="62"/>
       <c r="B25" s="56"/>
       <c r="C25" s="54"/>
       <c r="D25" s="56"/>
       <c r="E25" s="54"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="75"/>
+      <c r="A26" s="62"/>
       <c r="B26" s="56"/>
       <c r="C26" s="54"/>
       <c r="D26" s="56"/>
       <c r="E26" s="54"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="75"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="56"/>
       <c r="C27" s="54"/>
       <c r="D27" s="56"/>
       <c r="E27" s="54"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="75"/>
+      <c r="A28" s="62"/>
       <c r="B28" s="56"/>
       <c r="C28" s="54"/>
       <c r="D28" s="56"/>
       <c r="E28" s="54"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="75"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="56"/>
       <c r="C29" s="54"/>
       <c r="D29" s="56"/>
       <c r="E29" s="54"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="75"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="56"/>
       <c r="C30" s="54"/>
       <c r="D30" s="56"/>
       <c r="E30" s="54"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="75"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="56"/>
       <c r="C31" s="54"/>
       <c r="D31" s="56"/>
       <c r="E31" s="54"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="75"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="56"/>
       <c r="C32" s="54"/>
       <c r="D32" s="56"/>
       <c r="E32" s="54"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="75"/>
+      <c r="A33" s="62"/>
       <c r="B33" s="56"/>
       <c r="C33" s="54"/>
       <c r="D33" s="56"/>
       <c r="E33" s="54"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="75"/>
+      <c r="A34" s="62"/>
       <c r="B34" s="56"/>
       <c r="C34" s="54"/>
       <c r="D34" s="56"/>
       <c r="E34" s="54"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="75"/>
+      <c r="A35" s="62"/>
       <c r="B35" s="56"/>
       <c r="C35" s="54"/>
       <c r="D35" s="56"/>
       <c r="E35" s="54"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="75"/>
+      <c r="A36" s="62"/>
       <c r="B36" s="56"/>
       <c r="C36" s="54"/>
       <c r="D36" s="56"/>
       <c r="E36" s="54"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="75"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="56"/>
       <c r="C37" s="54"/>
       <c r="D37" s="56"/>
       <c r="E37" s="54"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="75"/>
+      <c r="A38" s="62"/>
       <c r="B38" s="56"/>
       <c r="C38" s="54"/>
       <c r="D38" s="56"/>
       <c r="E38" s="54"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="77"/>
+      <c r="A39" s="64"/>
       <c r="B39" s="57"/>
       <c r="C39" s="55"/>
       <c r="D39" s="56"/>
@@ -2368,8 +2366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1D5354-2649-42F7-ADA3-87EF3768865B}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2384,9 +2382,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="62">
+      <c r="A1" s="61">
         <f ca="1">NOW()</f>
-        <v>45334.053180439812</v>
+        <v>45335.068531712961</v>
       </c>
       <c r="B1" s="56">
         <v>80192</v>
@@ -2402,21 +2400,21 @@
       <c r="A2" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="72" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72" t="s">
+      <c r="E2" s="74"/>
+      <c r="F2" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="72"/>
+      <c r="G2" s="74"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="61"/>
+      <c r="A3" s="62"/>
       <c r="B3" s="56">
         <v>29624</v>
       </c>
@@ -2440,7 +2438,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="61">
+      <c r="A4" s="62">
         <v>45334.050180092592</v>
       </c>
       <c r="B4" s="56">
@@ -2461,333 +2459,645 @@
         <v>315500</v>
       </c>
       <c r="G4" s="59">
-        <f>F4/$D$1</f>
-        <v>4.81414794921875</v>
+        <f t="shared" ref="G4:G39" si="0">F4/$F$1</f>
+        <v>0.30088424682617188</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
-      <c r="B5" s="56"/>
+      <c r="A5" s="62">
+        <v>45335.066202314818</v>
+      </c>
+      <c r="B5" s="56">
+        <v>32608</v>
+      </c>
       <c r="C5" s="59">
         <f>B5/$B$1</f>
-        <v>0</v>
+        <v>0.40662410215482842</v>
       </c>
       <c r="D5" s="56"/>
       <c r="E5" s="59">
         <f>D5/$D$1</f>
         <v>0</v>
       </c>
-      <c r="F5" s="56"/>
+      <c r="F5" s="56">
+        <v>316588</v>
+      </c>
       <c r="G5" s="59">
-        <f>F5/$D$1</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.30192184448242188</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="56"/>
-      <c r="C6" s="59"/>
+      <c r="C6" s="59">
+        <f t="shared" ref="C6:C39" si="1">B6/$B$1</f>
+        <v>0</v>
+      </c>
       <c r="D6" s="56"/>
-      <c r="E6" s="59"/>
+      <c r="E6" s="59">
+        <f t="shared" ref="E6:E39" si="2">D6/$D$1</f>
+        <v>0</v>
+      </c>
       <c r="F6" s="56"/>
-      <c r="G6" s="59"/>
+      <c r="G6" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="61"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="56"/>
-      <c r="C7" s="59"/>
+      <c r="C7" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D7" s="56"/>
-      <c r="E7" s="59"/>
+      <c r="E7" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F7" s="56"/>
-      <c r="G7" s="59"/>
+      <c r="G7" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="61"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="56"/>
-      <c r="C8" s="59"/>
+      <c r="C8" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D8" s="56"/>
-      <c r="E8" s="59"/>
+      <c r="E8" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F8" s="56"/>
-      <c r="G8" s="59"/>
+      <c r="G8" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
+      <c r="A9" s="62"/>
       <c r="B9" s="56"/>
-      <c r="C9" s="59"/>
+      <c r="C9" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D9" s="56"/>
-      <c r="E9" s="59"/>
+      <c r="E9" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F9" s="56"/>
-      <c r="G9" s="59"/>
+      <c r="G9" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="56"/>
-      <c r="C10" s="59"/>
+      <c r="C10" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D10" s="56"/>
-      <c r="E10" s="59"/>
+      <c r="E10" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F10" s="56"/>
-      <c r="G10" s="59"/>
+      <c r="G10" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="61"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="56"/>
-      <c r="C11" s="59"/>
+      <c r="C11" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D11" s="56"/>
-      <c r="E11" s="59"/>
+      <c r="E11" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F11" s="56"/>
-      <c r="G11" s="59"/>
+      <c r="G11" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="56"/>
-      <c r="C12" s="59"/>
+      <c r="C12" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D12" s="56"/>
-      <c r="E12" s="59"/>
+      <c r="E12" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F12" s="56"/>
-      <c r="G12" s="59"/>
+      <c r="G12" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="56"/>
-      <c r="C13" s="59"/>
+      <c r="C13" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D13" s="56"/>
-      <c r="E13" s="59"/>
+      <c r="E13" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F13" s="56"/>
-      <c r="G13" s="59"/>
+      <c r="G13" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="61"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="56"/>
-      <c r="C14" s="59"/>
+      <c r="C14" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D14" s="56"/>
-      <c r="E14" s="59"/>
+      <c r="E14" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F14" s="56"/>
-      <c r="G14" s="59"/>
+      <c r="G14" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="56"/>
-      <c r="C15" s="59"/>
+      <c r="C15" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D15" s="56"/>
-      <c r="E15" s="59"/>
+      <c r="E15" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F15" s="56"/>
-      <c r="G15" s="59"/>
+      <c r="G15" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="61"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="56"/>
-      <c r="C16" s="59"/>
+      <c r="C16" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D16" s="56"/>
-      <c r="E16" s="59"/>
+      <c r="E16" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F16" s="56"/>
-      <c r="G16" s="59"/>
+      <c r="G16" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="61"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="56"/>
-      <c r="C17" s="59"/>
+      <c r="C17" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D17" s="56"/>
-      <c r="E17" s="59"/>
+      <c r="E17" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F17" s="56"/>
-      <c r="G17" s="59"/>
+      <c r="G17" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="61"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="56"/>
-      <c r="C18" s="59"/>
+      <c r="C18" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D18" s="56"/>
-      <c r="E18" s="59"/>
+      <c r="E18" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F18" s="56"/>
-      <c r="G18" s="59"/>
+      <c r="G18" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="56"/>
-      <c r="C19" s="59"/>
+      <c r="C19" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D19" s="56"/>
-      <c r="E19" s="59"/>
+      <c r="E19" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F19" s="56"/>
-      <c r="G19" s="59"/>
+      <c r="G19" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="61"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="56"/>
-      <c r="C20" s="59"/>
+      <c r="C20" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D20" s="56"/>
-      <c r="E20" s="59"/>
+      <c r="E20" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F20" s="56"/>
-      <c r="G20" s="59"/>
+      <c r="G20" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="61"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="56"/>
-      <c r="C21" s="59"/>
+      <c r="C21" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D21" s="56"/>
-      <c r="E21" s="59"/>
+      <c r="E21" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F21" s="56"/>
-      <c r="G21" s="59"/>
+      <c r="G21" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="61"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="56"/>
-      <c r="C22" s="59"/>
+      <c r="C22" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D22" s="56"/>
-      <c r="E22" s="59"/>
+      <c r="E22" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F22" s="56"/>
-      <c r="G22" s="59"/>
+      <c r="G22" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="61"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="56"/>
-      <c r="C23" s="59"/>
+      <c r="C23" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D23" s="56"/>
-      <c r="E23" s="59"/>
+      <c r="E23" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F23" s="56"/>
-      <c r="G23" s="59"/>
+      <c r="G23" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="61"/>
+      <c r="A24" s="62"/>
       <c r="B24" s="56"/>
-      <c r="C24" s="59"/>
+      <c r="C24" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D24" s="56"/>
-      <c r="E24" s="59"/>
+      <c r="E24" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F24" s="56"/>
-      <c r="G24" s="59"/>
+      <c r="G24" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="61"/>
+      <c r="A25" s="62"/>
       <c r="B25" s="56"/>
-      <c r="C25" s="59"/>
+      <c r="C25" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D25" s="56"/>
-      <c r="E25" s="59"/>
+      <c r="E25" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F25" s="56"/>
-      <c r="G25" s="59"/>
+      <c r="G25" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="61"/>
+      <c r="A26" s="62"/>
       <c r="B26" s="56"/>
-      <c r="C26" s="59"/>
+      <c r="C26" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D26" s="56"/>
-      <c r="E26" s="59"/>
+      <c r="E26" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F26" s="56"/>
-      <c r="G26" s="59"/>
+      <c r="G26" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="61"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="56"/>
-      <c r="C27" s="59"/>
+      <c r="C27" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D27" s="56"/>
-      <c r="E27" s="59"/>
+      <c r="E27" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F27" s="56"/>
-      <c r="G27" s="59"/>
+      <c r="G27" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="61"/>
+      <c r="A28" s="62"/>
       <c r="B28" s="56"/>
-      <c r="C28" s="59"/>
+      <c r="C28" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D28" s="56"/>
-      <c r="E28" s="59"/>
+      <c r="E28" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F28" s="56"/>
-      <c r="G28" s="59"/>
+      <c r="G28" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="56"/>
-      <c r="C29" s="59"/>
+      <c r="C29" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D29" s="56"/>
-      <c r="E29" s="59"/>
+      <c r="E29" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F29" s="56"/>
-      <c r="G29" s="59"/>
+      <c r="G29" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="61"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="56"/>
-      <c r="C30" s="59"/>
+      <c r="C30" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D30" s="56"/>
-      <c r="E30" s="59"/>
+      <c r="E30" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F30" s="56"/>
-      <c r="G30" s="59"/>
+      <c r="G30" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="61"/>
+      <c r="A31" s="62"/>
       <c r="B31" s="56"/>
-      <c r="C31" s="59"/>
+      <c r="C31" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D31" s="56"/>
-      <c r="E31" s="59"/>
+      <c r="E31" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F31" s="56"/>
-      <c r="G31" s="59"/>
+      <c r="G31" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="61"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="56"/>
-      <c r="C32" s="59"/>
+      <c r="C32" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D32" s="56"/>
-      <c r="E32" s="59"/>
+      <c r="E32" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F32" s="56"/>
-      <c r="G32" s="59"/>
+      <c r="G32" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="61"/>
+      <c r="A33" s="62"/>
       <c r="B33" s="56"/>
-      <c r="C33" s="59"/>
+      <c r="C33" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D33" s="56"/>
-      <c r="E33" s="59"/>
+      <c r="E33" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F33" s="56"/>
-      <c r="G33" s="59"/>
+      <c r="G33" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="61"/>
+      <c r="A34" s="62"/>
       <c r="B34" s="56"/>
-      <c r="C34" s="59"/>
+      <c r="C34" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D34" s="56"/>
-      <c r="E34" s="59"/>
+      <c r="E34" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F34" s="56"/>
-      <c r="G34" s="59"/>
+      <c r="G34" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="61"/>
+      <c r="A35" s="62"/>
       <c r="B35" s="56"/>
-      <c r="C35" s="59"/>
+      <c r="C35" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D35" s="56"/>
-      <c r="E35" s="59"/>
+      <c r="E35" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F35" s="56"/>
-      <c r="G35" s="59"/>
+      <c r="G35" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="61"/>
+      <c r="A36" s="62"/>
       <c r="B36" s="56"/>
-      <c r="C36" s="59"/>
+      <c r="C36" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D36" s="56"/>
-      <c r="E36" s="59"/>
+      <c r="E36" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F36" s="56"/>
-      <c r="G36" s="59"/>
+      <c r="G36" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="61"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="56"/>
-      <c r="C37" s="59"/>
+      <c r="C37" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D37" s="56"/>
-      <c r="E37" s="59"/>
+      <c r="E37" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F37" s="56"/>
-      <c r="G37" s="59"/>
+      <c r="G37" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="61"/>
+      <c r="A38" s="62"/>
       <c r="B38" s="56"/>
-      <c r="C38" s="59"/>
+      <c r="C38" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D38" s="56"/>
-      <c r="E38" s="59"/>
+      <c r="E38" s="59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F38" s="56"/>
-      <c r="G38" s="59"/>
+      <c r="G38" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="74"/>
-      <c r="B39" s="56"/>
-      <c r="C39" s="60"/>
+      <c r="A39" s="64"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="D39" s="57"/>
-      <c r="E39" s="60"/>
+      <c r="E39" s="60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F39" s="57"/>
-      <c r="G39" s="60"/>
+      <c r="G39" s="60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
SmartClockWeb8266: add russian font comments
</commit_message>
<xml_diff>
--- a/arduino/ФСА для ALI магазин.xlsx
+++ b/arduino/ФСА для ALI магазин.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arduino\arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42230DE9-2C8F-4FE8-B3AD-2EA574543CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1249B5D4-E591-4914-B530-4E2D5FB9639D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2034,7 +2034,7 @@
     <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="63">
         <f ca="1">NOW()</f>
-        <v>45351.054019560186</v>
+        <v>45357.960762615738</v>
       </c>
       <c r="B1" s="56">
         <v>1310720</v>
@@ -2391,7 +2391,7 @@
     <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="63">
         <f ca="1">NOW()</f>
-        <v>45351.054019560186</v>
+        <v>45357.960762615738</v>
       </c>
       <c r="B1" s="56">
         <v>80192</v>
@@ -2617,21 +2617,27 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="61"/>
-      <c r="B11" s="56"/>
+      <c r="A11" s="61">
+        <v>45357.960254745369</v>
+      </c>
+      <c r="B11" s="56">
+        <v>37600</v>
+      </c>
       <c r="C11" s="59">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.46887470071827614</v>
       </c>
       <c r="D11" s="56"/>
       <c r="E11" s="59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F11" s="56"/>
+      <c r="F11" s="56">
+        <v>350808</v>
+      </c>
       <c r="G11" s="59">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33455657958984375</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
SmartClockWeb8266: TFT_eSPI version to 2.5.43
</commit_message>
<xml_diff>
--- a/arduino/ФСА для ALI магазин.xlsx
+++ b/arduino/ФСА для ALI магазин.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arduino\arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1249B5D4-E591-4914-B530-4E2D5FB9639D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEC02C6-1838-4020-B56F-8265BB0E478D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2034,7 +2034,7 @@
     <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="63">
         <f ca="1">NOW()</f>
-        <v>45357.960762615738</v>
+        <v>45370.003913310182</v>
       </c>
       <c r="B1" s="56">
         <v>1310720</v>
@@ -2374,7 +2374,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2391,7 +2391,7 @@
     <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="63">
         <f ca="1">NOW()</f>
-        <v>45357.960762615738</v>
+        <v>45370.003913310182</v>
       </c>
       <c r="B1" s="56">
         <v>80192</v>
@@ -2641,21 +2641,29 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
-      <c r="B12" s="56"/>
+      <c r="A12" s="61">
+        <v>45370.003228935188</v>
+      </c>
+      <c r="B12" s="56">
+        <v>37412</v>
+      </c>
       <c r="C12" s="59">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="56"/>
+        <v>0.46653032721468474</v>
+      </c>
+      <c r="D12" s="56">
+        <v>61103</v>
+      </c>
       <c r="E12" s="59">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="56"/>
+        <v>0.9323577880859375</v>
+      </c>
+      <c r="F12" s="56">
+        <v>350632</v>
+      </c>
       <c r="G12" s="59">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33438873291015625</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>